<commit_message>
fix: currency enum (#46)
</commit_message>
<xml_diff>
--- a/Excel.output.xlsx
+++ b/Excel.output.xlsx
@@ -559,7 +559,7 @@
         <v>15000</v>
       </c>
       <c r="Q2" t="str">
-        <v>RUR</v>
+        <v>RUB</v>
       </c>
       <c r="R2" t="str">
         <v>01.01.2020</v>
@@ -684,7 +684,7 @@
         <v>15000</v>
       </c>
       <c r="Q3" t="str">
-        <v>RUR</v>
+        <v>RUB</v>
       </c>
       <c r="R3" t="str">
         <v>01.01.2020</v>

</xml_diff>